<commit_message>
uniting rows for insurer name in excel_download
</commit_message>
<xml_diff>
--- a/templates/summary_template.xlsx
+++ b/templates/summary_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grachev\Yandex.Disk\Работа\ОнлайнБрокер\soft\onlineservice\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7930D1A2-4D62-4919-A90A-464F38593855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A3E913-F969-4EF5-93AA-B22D446422A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -517,62 +517,65 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="3" fontId="12" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1739,8 +1742,8 @@
   </sheetPr>
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10:O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1766,69 +1769,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="3"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="63"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="55"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="52" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="5"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="65"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="57"/>
     </row>
     <row r="3" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="52" t="s">
+      <c r="B3" s="59"/>
+      <c r="C3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -1866,15 +1869,15 @@
       <c r="T4" s="8"/>
     </row>
     <row r="5" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -1916,23 +1919,23 @@
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="47" t="s">
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="62" t="s">
         <v>8</v>
       </c>
       <c r="J7" s="15"/>
-      <c r="K7" s="47" t="s">
+      <c r="K7" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="47" t="s">
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="62" t="s">
         <v>8</v>
       </c>
       <c r="P7" s="15"/>
@@ -1964,7 +1967,7 @@
       <c r="H8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="48"/>
+      <c r="I8" s="63"/>
       <c r="J8" s="18"/>
       <c r="K8" s="17" t="s">
         <v>13</v>
@@ -1978,7 +1981,7 @@
       <c r="N8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="48"/>
+      <c r="O8" s="63"/>
       <c r="P8" s="18"/>
       <c r="Q8" s="19" t="s">
         <v>17</v>
@@ -2033,7 +2036,7 @@
       <c r="H10" s="30">
         <v>1</v>
       </c>
-      <c r="I10" s="49">
+      <c r="I10" s="47">
         <f>SUM(F10:F12)</f>
         <v>293000</v>
       </c>
@@ -2051,7 +2054,7 @@
       <c r="N10" s="34">
         <v>1</v>
       </c>
-      <c r="O10" s="49">
+      <c r="O10" s="47">
         <f>SUM(L10:L12)</f>
         <v>217000</v>
       </c>
@@ -2085,7 +2088,7 @@
       <c r="H11" s="30">
         <v>1</v>
       </c>
-      <c r="I11" s="49"/>
+      <c r="I11" s="66"/>
       <c r="J11" s="37"/>
       <c r="K11" s="31">
         <f>L11/C11</f>
@@ -2100,7 +2103,7 @@
       <c r="N11" s="34">
         <v>1</v>
       </c>
-      <c r="O11" s="49"/>
+      <c r="O11" s="47"/>
       <c r="P11" s="37"/>
       <c r="Q11" s="38"/>
       <c r="R11" s="37"/>
@@ -2129,7 +2132,7 @@
       <c r="H12" s="30">
         <v>1</v>
       </c>
-      <c r="I12" s="49"/>
+      <c r="I12" s="66"/>
       <c r="J12" s="37"/>
       <c r="K12" s="31">
         <f>L12/C12</f>
@@ -2144,7 +2147,7 @@
       <c r="N12" s="34">
         <v>1</v>
       </c>
-      <c r="O12" s="49"/>
+      <c r="O12" s="47"/>
       <c r="P12" s="37"/>
       <c r="Q12" s="38"/>
       <c r="R12" s="37"/>
@@ -2196,22 +2199,20 @@
       <c r="T14" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="13">
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="I7:I8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="K1:N2"/>
     <mergeCell ref="S1:T2"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:G2"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="O10:O12"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="I7:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
consolidate comment section in excel_download
</commit_message>
<xml_diff>
--- a/templates/summary_template.xlsx
+++ b/templates/summary_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grachev\Yandex.Disk\Работа\ОнлайнБрокер\soft\onlineservice\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A3E913-F969-4EF5-93AA-B22D446422A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A731A9-5373-42B3-A381-A917419E5EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Свод котировок и условий по заявке №</t>
   </si>
@@ -83,15 +83,6 @@
     <t>1 год</t>
   </si>
   <si>
-    <t>Берут только при наличии штатной противоугонной системы.</t>
-  </si>
-  <si>
-    <t>2 год</t>
-  </si>
-  <si>
-    <t>3 год</t>
-  </si>
-  <si>
     <t>Технические данные</t>
   </si>
   <si>
@@ -117,6 +108,9 @@
   </si>
   <si>
     <t>Текст письма:</t>
+  </si>
+  <si>
+    <t>test comment</t>
   </si>
 </sst>
 </file>
@@ -407,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -500,14 +494,8 @@
     <xf numFmtId="49" fontId="14" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -520,6 +508,30 @@
     <xf numFmtId="3" fontId="12" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -549,33 +561,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1740,10 +1725,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10:O12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1769,69 +1754,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="50" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="3"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="55"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="61"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="60" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="5"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="57"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="63"/>
     </row>
     <row r="3" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="60" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -1869,15 +1854,15 @@
       <c r="T4" s="8"/>
     </row>
     <row r="5" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -1919,23 +1904,23 @@
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="62" t="s">
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="46" t="s">
         <v>8</v>
       </c>
       <c r="J7" s="15"/>
-      <c r="K7" s="62" t="s">
+      <c r="K7" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="63"/>
-      <c r="M7" s="63"/>
-      <c r="N7" s="63"/>
-      <c r="O7" s="62" t="s">
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="46" t="s">
         <v>8</v>
       </c>
       <c r="P7" s="15"/>
@@ -1967,7 +1952,7 @@
       <c r="H8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="63"/>
+      <c r="I8" s="47"/>
       <c r="J8" s="18"/>
       <c r="K8" s="17" t="s">
         <v>13</v>
@@ -1981,7 +1966,7 @@
       <c r="N8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="63"/>
+      <c r="O8" s="47"/>
       <c r="P8" s="18"/>
       <c r="Q8" s="19" t="s">
         <v>17</v>
@@ -2007,12 +1992,12 @@
       <c r="N9" s="22"/>
       <c r="O9" s="22"/>
       <c r="P9" s="27"/>
-      <c r="Q9" s="37"/>
+      <c r="Q9" s="36"/>
       <c r="R9" s="27"/>
       <c r="S9" s="7"/>
       <c r="T9" s="23"/>
     </row>
-    <row r="10" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="26.25" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
         <v>18</v>
       </c>
@@ -2036,9 +2021,9 @@
       <c r="H10" s="30">
         <v>1</v>
       </c>
-      <c r="I10" s="47">
-        <f>SUM(F10:F12)</f>
-        <v>293000</v>
+      <c r="I10" s="45">
+        <f>SUM(F10:F10)</f>
+        <v>100000</v>
       </c>
       <c r="J10" s="27"/>
       <c r="K10" s="31">
@@ -2054,152 +2039,48 @@
       <c r="N10" s="34">
         <v>1</v>
       </c>
-      <c r="O10" s="47">
-        <f>SUM(L10:L12)</f>
-        <v>217000</v>
+      <c r="O10" s="45">
+        <f>SUM(L10:L10)</f>
+        <v>75000</v>
       </c>
       <c r="P10" s="27"/>
       <c r="Q10" s="35" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="R10" s="27"/>
       <c r="S10" s="7"/>
       <c r="T10" s="23"/>
     </row>
-    <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
-      <c r="B11" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="26">
-        <v>2000000</v>
-      </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="28">
-        <f>F11/C11</f>
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="F11" s="29">
-        <v>98000</v>
-      </c>
-      <c r="G11" s="30">
-        <v>0</v>
-      </c>
-      <c r="H11" s="30">
-        <v>1</v>
-      </c>
-      <c r="I11" s="66"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="31">
-        <f>L11/C11</f>
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="L11" s="32">
-        <v>72000</v>
-      </c>
-      <c r="M11" s="33">
-        <v>50000</v>
-      </c>
-      <c r="N11" s="34">
-        <v>1</v>
-      </c>
-      <c r="O11" s="47"/>
-      <c r="P11" s="37"/>
+    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="37"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
-      <c r="R11" s="37"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="8"/>
-    </row>
-    <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
-      <c r="B12" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="26">
-        <v>2000000</v>
-      </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="28">
-        <f>F12/C12</f>
-        <v>4.7500000000000001E-2</v>
-      </c>
-      <c r="F12" s="29">
-        <v>95000</v>
-      </c>
-      <c r="G12" s="30">
-        <v>0</v>
-      </c>
-      <c r="H12" s="30">
-        <v>1</v>
-      </c>
-      <c r="I12" s="66"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="31">
-        <f>L12/C12</f>
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="L12" s="32">
-        <v>70000</v>
-      </c>
-      <c r="M12" s="33">
-        <v>50000</v>
-      </c>
-      <c r="N12" s="34">
-        <v>1</v>
-      </c>
-      <c r="O12" s="47"/>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="8"/>
-    </row>
-    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="8"/>
-    </row>
-    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="39"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="40"/>
-      <c r="R14" s="40"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="42"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="39"/>
+      <c r="T11" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="K1:N2"/>
+    <mergeCell ref="S1:T2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:G2"/>
     <mergeCell ref="O7:O8"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:G3"/>
@@ -2207,12 +2088,6 @@
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="K7:N7"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="K1:N2"/>
-    <mergeCell ref="S1:T2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -2238,288 +2113,288 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="42"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46" t="s">
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="46" t="s">
+      <c r="B7" s="42"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="42"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="42"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="46" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="44"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
+      <c r="B12" s="42"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="42"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="44"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="44"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="44"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="44"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="44"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="44"/>
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="44"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="44"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
+      <c r="A25" s="42"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="44"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="44"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
+      <c r="A27" s="42"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
+      <c r="A28" s="42"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="44"/>
-      <c r="B29" s="44"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
-      <c r="B30" s="44"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="44"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="44"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="44"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
+      <c r="A33" s="42"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="44"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="44"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
+      <c r="A35" s="42"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="44"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
+      <c r="A36" s="42"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="44"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="44"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add tech_info to excel_download
</commit_message>
<xml_diff>
--- a/templates/summary_template.xlsx
+++ b/templates/summary_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grachev\Yandex.Disk\Работа\ОнлайнБрокер\soft\onlineservice\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A731A9-5373-42B3-A381-A917419E5EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1323C567-9EBF-4798-841F-61CAEDAE922B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,7 +110,7 @@
     <t>Текст письма:</t>
   </si>
   <si>
-    <t>test comment</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -508,59 +508,59 @@
     <xf numFmtId="3" fontId="12" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1727,7 +1727,7 @@
   </sheetPr>
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
@@ -1754,69 +1754,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="56" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="3"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="61"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="53"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="5"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="63"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="55"/>
     </row>
     <row r="3" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="50" t="s">
+      <c r="B3" s="57"/>
+      <c r="C3" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -1854,15 +1854,15 @@
       <c r="T4" s="8"/>
     </row>
     <row r="5" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -1904,23 +1904,23 @@
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="46" t="s">
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="60" t="s">
         <v>8</v>
       </c>
       <c r="J7" s="15"/>
-      <c r="K7" s="46" t="s">
+      <c r="K7" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="46" t="s">
+      <c r="L7" s="61"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="60" t="s">
         <v>8</v>
       </c>
       <c r="P7" s="15"/>
@@ -1952,7 +1952,7 @@
       <c r="H8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="47"/>
+      <c r="I8" s="61"/>
       <c r="J8" s="18"/>
       <c r="K8" s="17" t="s">
         <v>13</v>
@@ -1966,7 +1966,7 @@
       <c r="N8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="47"/>
+      <c r="O8" s="61"/>
       <c r="P8" s="18"/>
       <c r="Q8" s="19" t="s">
         <v>17</v>
@@ -2075,12 +2075,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="K1:N2"/>
-    <mergeCell ref="S1:T2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:G2"/>
     <mergeCell ref="O7:O8"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:G3"/>
@@ -2088,6 +2082,12 @@
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="K7:N7"/>
     <mergeCell ref="I7:I8"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="K1:N2"/>
+    <mergeCell ref="S1:T2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
update aaditional values for property handling
</commit_message>
<xml_diff>
--- a/templates/summary_template.xlsx
+++ b/templates/summary_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grachev\Yandex.Disk\Работа\ОнлайнБрокер\soft\onlineservice\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255CFD10-0109-4222-8720-D01BFB6E887E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3523FD-555F-417D-A833-58D1D75D7387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary_template_sheet" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>Свод котировок и условий по заявке №</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Цели использования:</t>
   </si>
   <si>
-    <t>Дополнительные параметры запроса</t>
-  </si>
-  <si>
     <t>Автозапуск:</t>
   </si>
   <si>
@@ -149,14 +146,29 @@
     <t>Телематический комплекс:</t>
   </si>
   <si>
-    <t>будет дополнено позже</t>
+    <t>Доп. параметры для КАСКО\СТ</t>
+  </si>
+  <si>
+    <t>Территория страхования:</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Доп. параметры для имущества</t>
+  </si>
+  <si>
+    <t>Наличие перевозки:</t>
+  </si>
+  <si>
+    <t>Наличие СМР</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -198,13 +210,6 @@
       <u/>
       <sz val="14"/>
       <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -518,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -543,128 +548,79 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="15" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="14" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="15" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="14" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="17" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="16" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -673,32 +629,86 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="19" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="20" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="18" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="19" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="19" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="18" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="20" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="18" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="19" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="20" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="19" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1865,363 +1875,357 @@
   </sheetPr>
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="2.85546875" style="20" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="20" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="20" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="20" customWidth="1"/>
-    <col min="9" max="9" width="13" style="20" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" style="20" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" style="20" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="20" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="20" customWidth="1"/>
-    <col min="14" max="14" width="15" style="20" customWidth="1"/>
-    <col min="15" max="15" width="13" style="20" customWidth="1"/>
-    <col min="16" max="16" width="2.85546875" style="20" customWidth="1"/>
-    <col min="17" max="17" width="29.5703125" style="20" customWidth="1"/>
-    <col min="18" max="18" width="2.85546875" style="20" customWidth="1"/>
-    <col min="19" max="20" width="13.5703125" style="20" customWidth="1"/>
-    <col min="21" max="21" width="9" style="20" customWidth="1"/>
-    <col min="22" max="16384" width="9" style="20"/>
+    <col min="1" max="1" width="34.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" style="13" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="13" style="13" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" style="13" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" style="13" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="13" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="13" customWidth="1"/>
+    <col min="14" max="14" width="15" style="13" customWidth="1"/>
+    <col min="15" max="15" width="13" style="13" customWidth="1"/>
+    <col min="16" max="16" width="2.85546875" style="13" customWidth="1"/>
+    <col min="17" max="17" width="29.5703125" style="13" customWidth="1"/>
+    <col min="18" max="18" width="2.85546875" style="13" customWidth="1"/>
+    <col min="19" max="20" width="13.5703125" style="13" customWidth="1"/>
+    <col min="21" max="21" width="9" style="13" customWidth="1"/>
+    <col min="22" max="16384" width="9" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="19"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="60"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="29"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="61"/>
     </row>
     <row r="3" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23" t="s">
+      <c r="B3" s="63"/>
+      <c r="C3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="30"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="17"/>
     </row>
     <row r="4" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="30"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="17"/>
     </row>
     <row r="5" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="30"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="17"/>
     </row>
     <row r="6" spans="1:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="37"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="22"/>
     </row>
     <row r="7" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="40" t="s">
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="39"/>
-      <c r="K7" s="40" t="s">
+      <c r="J7" s="24"/>
+      <c r="K7" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="40" t="s">
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="37"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="22"/>
     </row>
     <row r="8" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="43" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="41"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="43" t="s">
+      <c r="I8" s="67"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="43" t="s">
+      <c r="L8" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="43" t="s">
+      <c r="M8" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="43" t="s">
+      <c r="N8" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="41"/>
-      <c r="P8" s="44"/>
-      <c r="Q8" s="45" t="s">
+      <c r="O8" s="67"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="R8" s="44"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="46"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="29"/>
     </row>
     <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="50"/>
-      <c r="R9" s="49"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="51"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="34"/>
     </row>
     <row r="10" spans="1:20" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="70">
+      <c r="C10" s="53">
         <v>2000000</v>
       </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="62">
+      <c r="D10" s="32"/>
+      <c r="E10" s="45">
         <f>F10/C10</f>
         <v>0.05</v>
       </c>
-      <c r="F10" s="63">
+      <c r="F10" s="46">
         <v>100000</v>
       </c>
-      <c r="G10" s="64">
+      <c r="G10" s="47">
         <v>0</v>
       </c>
-      <c r="H10" s="64">
+      <c r="H10" s="47">
         <v>1</v>
       </c>
-      <c r="I10" s="53">
+      <c r="I10" s="36">
         <f>SUM(F10:F10)</f>
         <v>100000</v>
       </c>
-      <c r="J10" s="49"/>
-      <c r="K10" s="65">
+      <c r="J10" s="32"/>
+      <c r="K10" s="48">
         <f>L10/C10</f>
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="L10" s="66">
+      <c r="L10" s="49">
         <v>75000</v>
       </c>
-      <c r="M10" s="67">
+      <c r="M10" s="50">
         <v>50000</v>
       </c>
-      <c r="N10" s="68">
+      <c r="N10" s="51">
         <v>1</v>
       </c>
-      <c r="O10" s="53">
+      <c r="O10" s="36">
         <f>SUM(L10:L10)</f>
         <v>75000</v>
       </c>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="54" t="s">
+      <c r="P10" s="32"/>
+      <c r="Q10" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="R10" s="49"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="51"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="34"/>
     </row>
     <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="55"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="56"/>
-      <c r="O11" s="56"/>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="56"/>
-      <c r="S11" s="56"/>
-      <c r="T11" s="57"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="39"/>
+      <c r="T11" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="K1:N2"/>
-    <mergeCell ref="S1:T2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:G2"/>
     <mergeCell ref="O7:O8"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:G3"/>
@@ -2229,6 +2233,12 @@
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="K7:N7"/>
     <mergeCell ref="I7:I8"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="K1:N2"/>
+    <mergeCell ref="S1:T2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="51" orientation="landscape" r:id="rId1"/>
@@ -2243,23 +2253,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.85546875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="76" style="11" customWidth="1"/>
-    <col min="3" max="3" width="9" style="11" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="11"/>
+    <col min="1" max="1" width="50.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="76" style="10" customWidth="1"/>
+    <col min="3" max="3" width="9" style="10" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
-    </row>
-    <row r="2" spans="1:2" s="11" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
+    </row>
+    <row r="2" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
@@ -2267,193 +2277,227 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="58"/>
-      <c r="B3" s="59"/>
-    </row>
-    <row r="4" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="59"/>
-      <c r="B9" s="59"/>
-    </row>
-    <row r="10" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="42"/>
+      <c r="B9" s="42"/>
+    </row>
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="70" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" s="11" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="60" t="s">
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="61"/>
-    </row>
-    <row r="13" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="11" customFormat="1" ht="143.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="143.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="61"/>
-    </row>
-    <row r="18" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="59"/>
-      <c r="B19" s="59"/>
-    </row>
-    <row r="20" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
+    </row>
+    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
+      <c r="B21" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="B22" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="41"/>
+      <c r="B25" s="42"/>
+    </row>
+    <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="58"/>
-      <c r="B25" s="59"/>
-    </row>
-    <row r="26" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
     </row>

</xml_diff>

<commit_message>
upd template generation - manufacturing_year, using_purposes, notes
</commit_message>
<xml_diff>
--- a/templates/summary_template.xlsx
+++ b/templates/summary_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grachev\Yandex.Disk\Работа\ОнлайнБрокер\soft\onlineservice\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961ED6AD-A7DD-411A-A742-E9F08FC986B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB6C746-7B03-4B5A-8310-30A394B72D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>Свод котировок и условий по заявке №</t>
   </si>
@@ -44,9 +44,6 @@
     <t>ООО "Ромашка"</t>
   </si>
   <si>
-    <t>Сводный сравнительный анализ котировок страховых тарифов и условий страхования</t>
-  </si>
-  <si>
     <t>Предложение 1</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>франшиза</t>
   </si>
   <si>
-    <t>рассрочка</t>
-  </si>
-  <si>
     <t>Комментарии</t>
   </si>
   <si>
@@ -168,13 +162,25 @@
   </si>
   <si>
     <t>Выбрано предложение:</t>
+  </si>
+  <si>
+    <t>Цели использования</t>
+  </si>
+  <si>
+    <t>Сравнительный анализ страховых тарифов</t>
+  </si>
+  <si>
+    <t>Примечание:</t>
+  </si>
+  <si>
+    <t>платежей в год</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -237,14 +243,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -331,6 +329,31 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
@@ -535,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -573,58 +596,51 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="8" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="14" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="13" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="14" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="13" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="16" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="15" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -638,31 +654,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="18" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="19" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="17" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="18" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="18" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="17" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="19" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="20" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="17" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="18" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="19" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="18" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -671,6 +687,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -707,28 +744,24 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1895,7 +1928,7 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="C3" sqref="C3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1924,71 +1957,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
       <c r="O1" s="12"/>
       <c r="P1" s="12"/>
-      <c r="Q1" s="72" t="s">
-        <v>46</v>
+      <c r="Q1" s="59" t="s">
+        <v>44</v>
       </c>
       <c r="R1" s="12"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="61"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="67"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="65" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
       <c r="O2" s="15"/>
       <c r="P2" s="15"/>
-      <c r="Q2" s="73"/>
+      <c r="Q2" s="52"/>
       <c r="R2" s="15"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="62"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="68"/>
     </row>
     <row r="3" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="65" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
@@ -1998,21 +2031,25 @@
       <c r="N3" s="14"/>
       <c r="O3" s="14"/>
       <c r="P3" s="14"/>
-      <c r="Q3" s="71" t="s">
-        <v>47</v>
+      <c r="Q3" s="60" t="s">
+        <v>45</v>
       </c>
       <c r="R3" s="14"/>
       <c r="S3" s="14"/>
       <c r="T3" s="16"/>
     </row>
-    <row r="4" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
+    <row r="4" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="70"/>
+      <c r="C4" s="75" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
@@ -2022,21 +2059,22 @@
       <c r="N4" s="14"/>
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
-      <c r="Q4" s="71"/>
+      <c r="Q4" s="53"/>
       <c r="R4" s="14"/>
       <c r="S4" s="14"/>
       <c r="T4" s="16"/>
     </row>
     <row r="5" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
+      <c r="B5" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="56"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
@@ -2046,217 +2084,220 @@
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
-      <c r="Q5" s="74"/>
+      <c r="Q5" s="54"/>
       <c r="R5" s="14"/>
       <c r="S5" s="14"/>
       <c r="T5" s="16"/>
     </row>
     <row r="6" spans="1:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
       <c r="R6" s="14"/>
       <c r="S6" s="14"/>
-      <c r="T6" s="21"/>
+      <c r="T6" s="19"/>
     </row>
     <row r="7" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="67" t="s">
+      <c r="A7" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="73" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="67" t="s">
+      <c r="J7" s="20"/>
+      <c r="K7" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="67" t="s">
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="19"/>
+    </row>
+    <row r="8" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="68"/>
-      <c r="M7" s="68"/>
-      <c r="N7" s="68"/>
-      <c r="O7" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="21"/>
-    </row>
-    <row r="8" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="B8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="C8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="D8" s="23"/>
+      <c r="E8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="25" t="s">
+      <c r="F8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="G8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="H8" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="74"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="O8" s="74"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="R8" s="23"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="25"/>
+    </row>
+    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="30"/>
+    </row>
+    <row r="10" spans="1:20" ht="26.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="68"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="N8" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="O8" s="68"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="27" t="s">
+      <c r="B10" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="R8" s="26"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="28"/>
-    </row>
-    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="33"/>
-    </row>
-    <row r="10" spans="1:20" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="52">
+      <c r="C10" s="49">
         <v>2000000</v>
       </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="44">
+      <c r="D10" s="28"/>
+      <c r="E10" s="41">
         <f>F10/C10</f>
         <v>0.05</v>
       </c>
-      <c r="F10" s="45">
+      <c r="F10" s="42">
         <v>100000</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="43">
         <v>0</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="43">
         <v>1</v>
       </c>
-      <c r="I10" s="35">
+      <c r="I10" s="32">
         <f>SUM(F10:F10)</f>
         <v>100000</v>
       </c>
-      <c r="J10" s="31"/>
-      <c r="K10" s="47">
+      <c r="J10" s="28"/>
+      <c r="K10" s="44">
         <f>L10/C10</f>
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="L10" s="48">
+      <c r="L10" s="45">
         <v>75000</v>
       </c>
-      <c r="M10" s="49">
+      <c r="M10" s="46">
         <v>50000</v>
       </c>
-      <c r="N10" s="50">
+      <c r="N10" s="47">
         <v>1</v>
       </c>
-      <c r="O10" s="35">
+      <c r="O10" s="32">
         <f>SUM(L10:L10)</f>
         <v>75000</v>
       </c>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="R10" s="31"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="R10" s="28"/>
       <c r="S10" s="14"/>
-      <c r="T10" s="33"/>
+      <c r="T10" s="30"/>
     </row>
     <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="39"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="Q3:Q4"/>
+  <mergeCells count="15">
     <mergeCell ref="O7:O8"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A5:G5"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="K7:N7"/>
     <mergeCell ref="I7:I8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A7:C7"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="K1:N2"/>
@@ -2265,7 +2306,7 @@
     <mergeCell ref="C2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="51" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="50" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Arial Cyr,Regular"&amp;10&amp;K000000summary_template.xlsx&amp;C&amp;"Helvetica Neue,Regular"&amp;11&amp;K000000&amp;P</oddHeader>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;11&amp;K000000&amp;P</oddFooter>
@@ -2290,123 +2331,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="40"/>
-      <c r="B1" s="40"/>
+      <c r="A1" s="37"/>
+      <c r="B1" s="37"/>
     </row>
     <row r="2" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40"/>
-      <c r="B3" s="41"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="38"/>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
-        <v>29</v>
+      <c r="A10" s="50" t="s">
+        <v>27</v>
       </c>
       <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>42</v>
+      <c r="A12" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="143.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="43" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2414,79 +2455,79 @@
       <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="38"/>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="54" t="s">
-        <v>40</v>
+      <c r="A20" s="51" t="s">
+        <v>38</v>
       </c>
       <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="40"/>
-      <c r="B25" s="41"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="38"/>
     </row>
     <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="54" t="s">
-        <v>43</v>
+      <c r="A26" s="51" t="s">
+        <v>41</v>
       </c>
       <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add manager name to ins_request
</commit_message>
<xml_diff>
--- a/templates/summary_template.xlsx
+++ b/templates/summary_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grachev\Yandex.Disk\Работа\ОнлайнБрокер\soft\onlineservice\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D29EDA6-7888-4D8D-9B0B-2A3AB541B0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13529FC-D95E-4AEE-8996-DCFD9EBFA04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary_template_sheet" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
     <t>Рассрочка:</t>
   </si>
   <si>
-    <t>Заправшиваемые риски:</t>
-  </si>
-  <si>
     <t>Банк-кредитор:</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>платежей в год</t>
+  </si>
+  <si>
+    <t>Запрашиваемые риски:</t>
   </si>
 </sst>
 </file>
@@ -716,6 +716,36 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -738,36 +768,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1935,7 +1935,7 @@
   </sheetPr>
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
@@ -1965,71 +1965,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
       <c r="O1" s="12"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R1" s="12"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="67"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="77"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="71" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
       <c r="O2" s="15"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="52"/>
       <c r="R2" s="15"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="68"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="78"/>
     </row>
     <row r="3" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="71" t="s">
+      <c r="B3" s="64"/>
+      <c r="C3" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
@@ -2040,24 +2040,24 @@
       <c r="O3" s="14"/>
       <c r="P3" s="14"/>
       <c r="Q3" s="58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R3" s="14"/>
       <c r="S3" s="14"/>
       <c r="T3" s="16"/>
     </row>
     <row r="4" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="75" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
+      <c r="A4" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="64"/>
+      <c r="C4" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
@@ -2074,10 +2074,10 @@
     </row>
     <row r="5" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="59" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="60" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="56"/>
       <c r="E5" s="55"/>
@@ -2120,29 +2120,29 @@
       <c r="T6" s="19"/>
     </row>
     <row r="7" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="77" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
+      <c r="A7" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="20"/>
-      <c r="E7" s="73" t="s">
+      <c r="E7" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="73" t="s">
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="61" t="s">
         <v>7</v>
       </c>
       <c r="J7" s="20"/>
-      <c r="K7" s="73" t="s">
+      <c r="K7" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="73" t="s">
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
+      <c r="O7" s="61" t="s">
         <v>7</v>
       </c>
       <c r="P7" s="20"/>
@@ -2172,9 +2172,9 @@
         <v>14</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="74"/>
+        <v>48</v>
+      </c>
+      <c r="I8" s="62"/>
       <c r="J8" s="23"/>
       <c r="K8" s="22" t="s">
         <v>12</v>
@@ -2186,9 +2186,9 @@
         <v>14</v>
       </c>
       <c r="N8" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="O8" s="74"/>
+        <v>48</v>
+      </c>
+      <c r="O8" s="62"/>
       <c r="P8" s="23"/>
       <c r="Q8" s="24" t="s">
         <v>15</v>
@@ -2297,6 +2297,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="K1:N2"/>
+    <mergeCell ref="S1:T2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:G2"/>
     <mergeCell ref="O7:O8"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:G3"/>
@@ -2306,12 +2312,6 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="K1:N2"/>
-    <mergeCell ref="S1:T2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" orientation="landscape" r:id="rId1"/>
@@ -2326,8 +2326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2365,7 +2365,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2373,7 +2373,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2381,7 +2381,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2389,7 +2389,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2407,7 +2407,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2415,15 +2415,15 @@
         <v>23</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2431,7 +2431,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2439,23 +2439,23 @@
         <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="143.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2468,40 +2468,40 @@
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2510,32 +2510,32 @@
     </row>
     <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>